<commit_message>
[FIX] add column asset_management
</commit_message>
<xml_diff>
--- a/rjc_account_asset_excel/report_asset/report_asset.xlsx
+++ b/rjc_account_asset_excel/report_asset/report_asset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t xml:space="preserve">Asset Report</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">อัตราร้อยละ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">มูลค่าที่คิดค่าเสื่อม</t>
   </si>
   <si>
     <t xml:space="preserve">ราคาซาก</t>
@@ -280,9 +283,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="20" min="20" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,6 +300,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
@@ -312,6 +316,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -327,6 +332,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
@@ -342,6 +348,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4"/>
@@ -383,22 +390,24 @@
       <c r="L6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="0"/>
+      <c r="M6" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="Q6" s="0"/>
       <c r="R6" s="0"/>
-      <c r="T6" s="5" t="s">
+      <c r="S6" s="0"/>
+      <c r="U6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AMG6" s="0"/>
       <c r="AMH6" s="0"/>
       <c r="AMI6" s="0"/>
       <c r="AMJ6" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
+  <mergeCells count="17">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
@@ -411,7 +420,8 @@
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:L7"/>
-    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="U6:U7"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>